<commit_message>
Uptade all the functions
</commit_message>
<xml_diff>
--- a/dados_ibge.xlsx
+++ b/dados_ibge.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,31 +451,135 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t xml:space="preserve">baiano
-</t>
+          <t>acriano</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Salvador
-</t>
+          <t>Rio Branco</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t xml:space="preserve">JERÔNIMO RODRIGUES SOUZA
-</t>
+          <t>GLADSON DE LIMA CAMELI</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t xml:space="preserve">14.985.284 </t>
+          <t>906.876</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t xml:space="preserve">0,660  
-</t>
+          <t>0,663</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>alagoano</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Maceió</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>PAULO SURUAGY DO AMARAL DANTAS</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>3.365.351</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>0,631</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>amapaense</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Macapá</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>CLÉCIO LUÍS VILHENA VIEIRA</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>877.613</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>0,708</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>amazonense</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Manaus</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>WILSON MIRANDA LIMA</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>4.269.995</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>0,674</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>baiano</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Salvador</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>JERÔNIMO RODRIGUES SOUZA</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>14.985.284</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>0,660</t>
         </is>
       </c>
     </row>

</xml_diff>